<commit_message>
Add integration of FTP/zero-is new for uniform integration
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.cat.resource.tree.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.cat.resource.tree.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE11C3DE-8C4A-D145-9DA8-FE635D0723B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F6311-550C-EE48-9F40-105A0BFB2CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73620" yWindow="-12580" windowWidth="34220" windowHeight="26580" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="63260" yWindow="-8400" windowWidth="34220" windowHeight="26580" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="209">
   <si>
     <t>code</t>
   </si>
@@ -780,6 +780,17 @@
   </si>
   <si>
     <t>psi.position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource.integration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5c744f47-471a-405c-b616-9b58b9f8ed03</t>
+  </si>
+  <si>
+    <t>集成服务管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1005,27 +1016,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1436,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500280C7-B0AC-7C45-9420-F2551253A777}">
-  <dimension ref="A2:I65"/>
+  <dimension ref="A2:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -1550,7 +1541,7 @@
         <v>21</v>
       </c>
       <c r="H5" s="21">
-        <v>1</v>
+        <v>1005</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>24</v>
@@ -1857,7 +1848,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="21">
-        <v>2</v>
+        <v>1010</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>24</v>
@@ -2108,7 +2099,7 @@
         <v>21</v>
       </c>
       <c r="H25" s="21">
-        <v>3</v>
+        <v>1015</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>24</v>
@@ -2283,18 +2274,18 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="66">
-      <c r="A32" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B32" s="8"/>
+      <c r="A32" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="17"/>
       <c r="C32" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="F32" s="19" t="b">
         <v>1</v>
@@ -2303,99 +2294,98 @@
         <v>21</v>
       </c>
       <c r="H32" s="21">
-        <v>4</v>
+        <v>1020</v>
       </c>
       <c r="I32" s="22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" ht="66">
       <c r="A33" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="8" t="str">
-        <f>A$32</f>
-        <v>89f2a233-3b52-4fd2-95e7-11a0dc0bdba8</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B33" s="8"/>
       <c r="C33" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>167</v>
+      <c r="D33" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>159</v>
       </c>
       <c r="F33" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="G33" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H33" s="24">
-        <v>1</v>
-      </c>
-      <c r="I33" s="13"/>
+      <c r="G33" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="21">
+        <v>1025</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B34" s="8" t="str">
-        <f t="shared" ref="B34:B39" si="4">A$32</f>
+        <f>A$33</f>
         <v>89f2a233-3b52-4fd2-95e7-11a0dc0bdba8</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H34" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B35:B40" si="4">A$33</f>
         <v>89f2a233-3b52-4fd2-95e7-11a0dc0bdba8</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F35" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H35" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="8" t="str">
         <f t="shared" si="4"/>
@@ -2405,25 +2395,25 @@
         <v>21</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F36" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H36" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" s="8" t="str">
         <f t="shared" si="4"/>
@@ -2433,25 +2423,25 @@
         <v>21</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F37" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H37" s="24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B38" s="8" t="str">
         <f t="shared" si="4"/>
@@ -2461,25 +2451,25 @@
         <v>21</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F38" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H38" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="8" t="str">
         <f t="shared" si="4"/>
@@ -2489,164 +2479,164 @@
         <v>21</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F39" s="19" t="b">
         <v>1</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H39" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>89f2a233-3b52-4fd2-95e7-11a0dc0bdba8</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="H40" s="24">
+        <v>7</v>
+      </c>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B40" s="8" t="str">
-        <f t="shared" ref="B40" si="5">A$32</f>
+      <c r="B41" s="8" t="str">
+        <f t="shared" ref="B41" si="5">A$33</f>
         <v>89f2a233-3b52-4fd2-95e7-11a0dc0bdba8</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="14" t="s">
+      <c r="C41" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E41" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="F40" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="23" t="s">
+      <c r="F41" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H41" s="24">
         <v>8</v>
       </c>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="66">
-      <c r="A41" s="16" t="s">
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="66">
+      <c r="A42" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="15" t="s">
+      <c r="B42" s="17"/>
+      <c r="C42" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="21">
-        <v>4</v>
-      </c>
-      <c r="I41" s="22" t="s">
+      <c r="F42" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="21">
+        <v>1030</v>
+      </c>
+      <c r="I42" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B42" s="8" t="str">
-        <f>A$41</f>
-        <v>15d054b3-db6f-4fd2-bcb2-51faa8daa746</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" s="24">
-        <v>1</v>
-      </c>
-      <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="8" t="str">
-        <f t="shared" ref="B43:B49" si="6">A$41</f>
+        <f>A$42</f>
         <v>15d054b3-db6f-4fd2-bcb2-51faa8daa746</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="F43" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="H43" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" s="13"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="B44:B50" si="6">A$42</f>
         <v>15d054b3-db6f-4fd2-bcb2-51faa8daa746</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="F44" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="H44" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I44" s="13"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B45" s="8" t="str">
         <f t="shared" si="6"/>
@@ -2656,25 +2646,25 @@
         <v>21</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F45" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H45" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B46" s="8" t="str">
         <f t="shared" si="6"/>
@@ -2684,25 +2674,25 @@
         <v>21</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="F46" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="H46" s="24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="8" t="str">
         <f t="shared" si="6"/>
@@ -2712,25 +2702,25 @@
         <v>21</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="F47" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="H47" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I47" s="13"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" s="8" t="str">
         <f t="shared" si="6"/>
@@ -2740,25 +2730,25 @@
         <v>21</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F48" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H48" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B49" s="8" t="str">
         <f t="shared" si="6"/>
@@ -2768,136 +2758,136 @@
         <v>21</v>
       </c>
       <c r="D49" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H49" s="24">
+        <v>7</v>
+      </c>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>15d054b3-db6f-4fd2-bcb2-51faa8daa746</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E50" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G49" s="10" t="s">
+      <c r="F50" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H49" s="24">
+      <c r="H50" s="24">
         <v>8</v>
       </c>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="1:9" ht="66">
-      <c r="A50" s="16" t="s">
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="66">
+      <c r="A51" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="15" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E51" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F50" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" s="21">
-        <v>5</v>
-      </c>
-      <c r="I50" s="22" t="s">
+      <c r="F51" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" s="21">
+        <v>1035</v>
+      </c>
+      <c r="I51" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="8" t="str">
-        <f>A$50</f>
-        <v>e391106f-8f49-4523-a662-d65859277e88</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F51" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H51" s="24">
-        <v>1</v>
-      </c>
-      <c r="I51" s="13"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="8" t="str">
-        <f t="shared" ref="B52:B57" si="7">A$50</f>
+        <f>A$51</f>
         <v>e391106f-8f49-4523-a662-d65859277e88</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F52" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H52" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="B53:B58" si="7">A$51</f>
         <v>e391106f-8f49-4523-a662-d65859277e88</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F53" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H53" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="8" t="str">
         <f t="shared" si="7"/>
@@ -2907,25 +2897,25 @@
         <v>21</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F54" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H54" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" s="8" t="str">
         <f t="shared" si="7"/>
@@ -2935,25 +2925,25 @@
         <v>21</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F55" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H55" s="24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="8" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="B56" s="8" t="str">
         <f t="shared" si="7"/>
@@ -2963,25 +2953,25 @@
         <v>21</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F56" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H56" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="8" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B57" s="8" t="str">
         <f t="shared" si="7"/>
@@ -2991,240 +2981,268 @@
         <v>21</v>
       </c>
       <c r="D57" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H57" s="24">
+        <v>6</v>
+      </c>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>e391106f-8f49-4523-a662-d65859277e88</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E58" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F57" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G57" s="23" t="s">
+      <c r="F58" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H58" s="24">
         <v>7</v>
       </c>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="1:9" ht="66">
-      <c r="A58" s="8" t="s">
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" ht="66">
+      <c r="A59" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="14" t="s">
+      <c r="B59" s="8"/>
+      <c r="C59" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="E58" s="23" t="s">
+      <c r="E59" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="F58" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G58" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" s="21">
-        <v>6</v>
-      </c>
-      <c r="I58" s="22" t="s">
+      <c r="F59" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="21">
+        <v>1040</v>
+      </c>
+      <c r="I59" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B59" s="8" t="str">
-        <f>A$58</f>
-        <v>4e68fe4f-7a49-43bd-90d7-fd90a6fced41</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="E59" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F59" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="H59" s="24">
-        <v>1</v>
-      </c>
-      <c r="I59" s="13"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B60" s="8" t="str">
-        <f t="shared" ref="B60:B61" si="8">A$58</f>
+        <f>A$59</f>
         <v>4e68fe4f-7a49-43bd-90d7-fd90a6fced41</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>188</v>
+        <v>93</v>
       </c>
       <c r="F60" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>188</v>
+        <v>93</v>
       </c>
       <c r="H60" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="8" t="str">
+        <f t="shared" ref="B61:B62" si="8">A$59</f>
+        <v>4e68fe4f-7a49-43bd-90d7-fd90a6fced41</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F61" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H61" s="24">
+        <v>2</v>
+      </c>
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B61" s="8" t="str">
+      <c r="B62" s="8" t="str">
         <f t="shared" si="8"/>
         <v>4e68fe4f-7a49-43bd-90d7-fd90a6fced41</v>
       </c>
-      <c r="C61" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="14" t="s">
+      <c r="C62" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="E61" s="23" t="s">
+      <c r="E62" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="F61" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G61" s="23" t="s">
+      <c r="F62" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="H61" s="24">
+      <c r="H62" s="24">
         <v>3</v>
       </c>
-      <c r="I61" s="13"/>
-    </row>
-    <row r="62" spans="1:9" ht="66">
-      <c r="A62" s="8" t="s">
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" ht="66">
+      <c r="A63" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="14" t="s">
+      <c r="B63" s="8"/>
+      <c r="C63" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="23" t="s">
+      <c r="E63" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="F62" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H62" s="21">
-        <v>7</v>
-      </c>
-      <c r="I62" s="22" t="s">
+      <c r="F63" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63" s="21">
+        <v>1045</v>
+      </c>
+      <c r="I63" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B63" s="8" t="str">
-        <f>A$62</f>
-        <v>0d059d25-90e2-46ed-93f5-093e27d37a8c</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E63" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F63" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="H63" s="24">
-        <v>1</v>
-      </c>
-      <c r="I63" s="13"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="8" t="str">
+        <f>A$63</f>
+        <v>0d059d25-90e2-46ed-93f5-093e27d37a8c</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="F64" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="H64" s="24">
+        <v>1</v>
+      </c>
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B64" s="8" t="str">
-        <f>A$62</f>
+      <c r="B65" s="8" t="str">
+        <f>A$63</f>
         <v>0d059d25-90e2-46ed-93f5-093e27d37a8c</v>
       </c>
-      <c r="C64" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D64" s="14" t="s">
+      <c r="C65" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="E64" s="23" t="s">
+      <c r="E65" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="F64" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G64" s="23" t="s">
+      <c r="F65" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="H64" s="24">
+      <c r="H65" s="24">
         <v>2</v>
       </c>
-      <c r="I64" s="13"/>
-    </row>
-    <row r="65" spans="1:9" ht="66">
-      <c r="A65" s="16" t="s">
+      <c r="I65" s="13"/>
+    </row>
+    <row r="66" spans="1:9" ht="66">
+      <c r="A66" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="15" t="s">
+      <c r="B66" s="17"/>
+      <c r="C66" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E66" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F65" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H65" s="21">
-        <v>8</v>
-      </c>
-      <c r="I65" s="22" t="s">
+      <c r="F66" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" s="21">
+        <v>1050</v>
+      </c>
+      <c r="I66" s="22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3233,23 +3251,15 @@
     <mergeCell ref="C2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1 F66:F1048576 F44:F45 F47:F56 F41:F42 F3:F31 F58:F64">
-    <cfRule type="cellIs" dxfId="11" priority="35" operator="equal">
+  <conditionalFormatting sqref="F1 F45:F46 F48:F57 F42:F43 F59:F1048576 F3:F32">
+    <cfRule type="cellIs" dxfId="9" priority="35" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="36" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F65">
-    <cfRule type="cellIs" dxfId="9" priority="33" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="34" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F57:F64">
+  <conditionalFormatting sqref="F58:F65">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -3257,7 +3267,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
+  <conditionalFormatting sqref="F44">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -3265,7 +3275,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
+  <conditionalFormatting sqref="F47">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -3273,7 +3283,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32:F40">
+  <conditionalFormatting sqref="F33:F41">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>